<commit_message>
Vincule tabla_contactos a ventanaPrincipal y agregue librerias en readme
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,79 +469,93 @@
           <t>Soni</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>3644680959</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3644123456</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>snhernandez6@gmail.com</t>
+          <t>srhernandez@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ant. Arg.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>cvc</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>vv</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>vv</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>bvb@gg.vo</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>vb</t>
+          <t>Bn 234</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>few</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>Sonia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ff</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>8888</v>
+          <t>Soni</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3644567800</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>gf@ee.com</t>
+          <t>shernandez@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>efew</t>
-        </is>
-      </c>
+          <t>Ant Arg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Graciela</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gra</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>34567890</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>gra12@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>La Rioja</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>